<commit_message>
Naming Convention and comments
</commit_message>
<xml_diff>
--- a/Excel/Data.xlsx
+++ b/Excel/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabha\Desktop\Prabha\Resumes\Applied Projects\Westpac_Assessment-master\Westpac_Assessment-master\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria.Sagayaraj\Desktop\Westpac_Assessment\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D414FBC-DA57-423D-87A1-D23675E6B007}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A42E7C-8C38-4ED8-AC88-CE148AE92F9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2655" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-3760" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="7" r:id="rId1"/>
@@ -91,9 +91,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>msa</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>Drawing</t>
+  </si>
+  <si>
+    <t>masa</t>
   </si>
 </sst>
 </file>
@@ -557,30 +557,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{560CE7BE-B73A-40BD-A9EC-02F85437864E}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.54296875" customWidth="1"/>
-    <col min="3" max="3" width="17.7265625" customWidth="1"/>
-    <col min="4" max="4" width="25.1796875" customWidth="1"/>
-    <col min="5" max="5" width="26.26953125" customWidth="1"/>
-    <col min="6" max="6" width="24.54296875" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" customWidth="1"/>
-    <col min="9" max="9" width="28.81640625" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="12" width="22.54296875" customWidth="1"/>
-    <col min="13" max="13" width="18.453125" customWidth="1"/>
-    <col min="14" max="14" width="22.453125" customWidth="1"/>
-    <col min="15" max="16" width="23.26953125" customWidth="1"/>
+    <col min="11" max="12" width="22.5703125" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" customWidth="1"/>
+    <col min="15" max="16" width="23.28515625" customWidth="1"/>
     <col min="17" max="17" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -615,7 +615,7 @@
         <v>12</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>15</v>
@@ -627,15 +627,15 @@
         <v>18</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="8" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" s="8" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>21</v>
@@ -663,7 +663,7 @@
         <v>14</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M2" s="8">
         <v>28</v>
@@ -675,13 +675,13 @@
         <v>2108060859</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q2" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -691,7 +691,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -701,7 +701,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -712,7 +712,7 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -723,7 +723,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -734,7 +734,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -745,7 +745,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -756,7 +756,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -767,7 +767,7 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -778,7 +778,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -789,7 +789,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -800,7 +800,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -811,7 +811,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -822,7 +822,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -833,7 +833,7 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -844,7 +844,7 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -855,7 +855,7 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -866,7 +866,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -877,7 +877,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -888,7 +888,7 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -899,7 +899,7 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -910,7 +910,7 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -921,7 +921,7 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -932,7 +932,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -943,7 +943,7 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -954,7 +954,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -965,7 +965,7 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -976,7 +976,7 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -987,7 +987,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>

</xml_diff>